<commit_message>
added database + activity diagram
</commit_message>
<xml_diff>
--- a/Documentation/UML Project check list.xlsx
+++ b/Documentation/UML Project check list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcovinciguerra/Github/SoftwareEngProject/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208BE9D8-569E-5F46-B5A6-BF7661B2FAF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CA3C04-44A9-DC40-A7B8-27B5977BCDCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="42">
   <si>
     <t>UML Project check list</t>
   </si>
@@ -569,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -920,13 +920,19 @@
       <c r="B48" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C48" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B49" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C49" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>2</v>
       </c>
@@ -934,17 +940,20 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B51" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B52" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C52" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>3</v>
       </c>
@@ -952,30 +961,42 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B54" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C54" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B55" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C55" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <v>4</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C56" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <v>5</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>40</v>
+      </c>
+      <c r="C57" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -993,6 +1014,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100ED38291D0B6A0B4F876ADAB3182D3E9F" ma:contentTypeVersion="9" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="0237eb97371f807641e5619f4bd3ffe6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="36d25196-f32b-43e1-8250-558e57115123" xmlns:ns3="ebc603f1-ec20-4f4d-b061-13224f8f2a67" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="29debb1426aedb772aa01b22e7a7180e" ns2:_="" ns3:_="">
     <xsd:import namespace="36d25196-f32b-43e1-8250-558e57115123"/>
@@ -1189,22 +1225,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B32DCA8-8641-4B2C-9DA8-CA33157E7EFE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0F56034-9203-419C-A3C7-A48D5210236D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E2B2261-019D-480F-A6F6-99B8B489586A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1221,21 +1259,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0F56034-9203-419C-A3C7-A48D5210236D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B32DCA8-8641-4B2C-9DA8-CA33157E7EFE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added activity diagram + updated project plan
</commit_message>
<xml_diff>
--- a/Documentation/UML Project check list.xlsx
+++ b/Documentation/UML Project check list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcovinciguerra/Github/SoftwareEngProject/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208BE9D8-569E-5F46-B5A6-BF7661B2FAF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B294F2-CB09-FE4F-B48B-434AA0A4FBE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="42">
   <si>
     <t>UML Project check list</t>
   </si>
@@ -569,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -920,13 +920,19 @@
       <c r="B48" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C48" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B49" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C49" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>2</v>
       </c>
@@ -934,35 +940,44 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B51" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B52" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C52" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>3</v>
       </c>
       <c r="B53" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C53" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B54" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C54" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B55" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <v>4</v>
       </c>
@@ -970,12 +985,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <v>5</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>40</v>
+      </c>
+      <c r="C57" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -993,6 +1011,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100ED38291D0B6A0B4F876ADAB3182D3E9F" ma:contentTypeVersion="9" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="0237eb97371f807641e5619f4bd3ffe6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="36d25196-f32b-43e1-8250-558e57115123" xmlns:ns3="ebc603f1-ec20-4f4d-b061-13224f8f2a67" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="29debb1426aedb772aa01b22e7a7180e" ns2:_="" ns3:_="">
     <xsd:import namespace="36d25196-f32b-43e1-8250-558e57115123"/>
@@ -1189,22 +1222,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B32DCA8-8641-4B2C-9DA8-CA33157E7EFE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0F56034-9203-419C-A3C7-A48D5210236D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E2B2261-019D-480F-A6F6-99B8B489586A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1221,21 +1256,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0F56034-9203-419C-A3C7-A48D5210236D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B32DCA8-8641-4B2C-9DA8-CA33157E7EFE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
dart classes + documentation
</commit_message>
<xml_diff>
--- a/Documentation/UML Project check list.xlsx
+++ b/Documentation/UML Project check list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcovinciguerra/Github/SoftwareEngProject/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B294F2-CB09-FE4F-B48B-434AA0A4FBE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5964275-909A-EE40-9A48-FE51C2516A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="43">
   <si>
     <t>UML Project check list</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>state machine diagram da sistemare</t>
   </si>
 </sst>
 </file>
@@ -276,13 +279,13 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -569,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -587,10 +590,10 @@
     </row>
     <row r="2" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="9"/>
+      <c r="B3" s="7"/>
       <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -662,10 +665,10 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="9"/>
+      <c r="B13" s="7"/>
       <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -755,10 +758,13 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="7"/>
+      <c r="B25" s="9"/>
+      <c r="C25" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="26" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
@@ -832,10 +838,10 @@
       </c>
     </row>
     <row r="37" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B37" s="7"/>
+      <c r="B37" s="9"/>
     </row>
     <row r="38" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
@@ -907,6 +913,7 @@
         <v>35</v>
       </c>
       <c r="B46" s="7"/>
+      <c r="C46" s="6"/>
     </row>
     <row r="47" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
@@ -915,6 +922,9 @@
       <c r="B47" t="s">
         <v>12</v>
       </c>
+      <c r="C47" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
@@ -939,19 +949,22 @@
       <c r="B50" t="s">
         <v>12</v>
       </c>
+      <c r="C50" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B51" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="C51" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B52" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C52" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
@@ -976,6 +989,9 @@
       <c r="B55" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="C55" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
@@ -983,6 +999,9 @@
       </c>
       <c r="B56" s="3" t="s">
         <v>39</v>
+      </c>
+      <c r="C56" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>